<commit_message>
debugged the reader script.
just input a number greater than 4 when it asks and it will print out the relevant info from each school on that row. I am very proud.
</commit_message>
<xml_diff>
--- a/outdoor.xlsx
+++ b/outdoor.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\qualtrics_data_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{79FC81AE-3536-4258-9FFC-AFA920013527}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0938037E-0022-49C2-8F9A-C886008C22BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outdoor" sheetId="1" r:id="rId1"/>
@@ -21976,7 +21976,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -22814,11 +22814,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CKD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
-      <selection activeCell="BG2" sqref="BG2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22852,11 +22852,22 @@
     <col min="54" max="54" width="81.28515625" customWidth="1"/>
     <col min="55" max="55" width="49.140625" customWidth="1"/>
     <col min="56" max="56" width="37.85546875" customWidth="1"/>
-    <col min="57" max="57" width="22.5703125" customWidth="1"/>
+    <col min="57" max="57" width="29.42578125" customWidth="1"/>
     <col min="58" max="58" width="11.42578125" customWidth="1"/>
     <col min="59" max="59" width="9.28515625" customWidth="1"/>
     <col min="62" max="62" width="37.5703125" customWidth="1"/>
-    <col min="63" max="63" width="64.42578125" customWidth="1"/>
+    <col min="63" max="63" width="79.42578125" customWidth="1"/>
+    <col min="224" max="224" width="63.42578125" customWidth="1"/>
+    <col min="247" max="247" width="64.85546875" customWidth="1"/>
+    <col min="270" max="270" width="67.7109375" customWidth="1"/>
+    <col min="500" max="500" width="63.42578125" customWidth="1"/>
+    <col min="730" max="730" width="65" customWidth="1"/>
+    <col min="960" max="960" width="68.28515625" customWidth="1"/>
+    <col min="1190" max="1190" width="63.42578125" customWidth="1"/>
+    <col min="1420" max="1420" width="62.85546875" customWidth="1"/>
+    <col min="1650" max="1650" width="64.140625" customWidth="1"/>
+    <col min="1880" max="1880" width="63.7109375" customWidth="1"/>
+    <col min="2110" max="2110" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2318" x14ac:dyDescent="0.25">

</xml_diff>